<commit_message>
Support multiple cards per entry.
</commit_message>
<xml_diff>
--- a/Test Cards.xlsx
+++ b/Test Cards.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Text can contain &lt;b&gt;HTML markup&lt;/b&gt; for better formatting, provided it's filtered through &lt;code&gt;safe&lt;/code&gt; in the Django template.</t>
+  </si>
+  <si>
+    <t>base,base</t>
   </si>
 </sst>
 </file>
@@ -446,7 +449,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -481,7 +484,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>

</xml_diff>